<commit_message>
Objectification of excel parser step 1
</commit_message>
<xml_diff>
--- a/server/prasignups.xlsx
+++ b/server/prasignups.xlsx
@@ -264,7 +264,7 @@
     <numFmt numFmtId="242" formatCode="$0.00"/>
     <numFmt numFmtId="243" formatCode="$0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +275,7 @@
     <font>
       <b/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -335,73 +336,73 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="185" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="186" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="187" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="188" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="191" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="192" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="193" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="196" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="197" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="199" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="200" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="202" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="203" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="204" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="205" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="189" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="190" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="191" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="192" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="193" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="194" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="195" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="196" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="197" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="198" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="199" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="200" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="201" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="202" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="203" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="204" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="205" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="206" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="207" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="209" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="210" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="211" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="212" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="213" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="214" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="207" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="208" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="209" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="210" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="211" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="212" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="213" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="214" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="215" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="216" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="217" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="218" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="219" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="220" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="218" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="219" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="220" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="221" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="222" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="223" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="224" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="225" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="226" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="227" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="228" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="229" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="230" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="231" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="232" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="233" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="234" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="235" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="236" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="237" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="238" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="239" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="240" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="241" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="242" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="243" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="222" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="223" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="224" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="225" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="226" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="227" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="228" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="229" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="230" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="231" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="232" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="233" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="234" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="235" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="236" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="237" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="238" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="239" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="240" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="241" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="242" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="243" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>